<commit_message>
change all the database and xlsx data schema to lower case due to postgres' features & fix the database connection problem
</commit_message>
<xml_diff>
--- a/epic.xlsx
+++ b/epic.xlsx
@@ -1,39 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27106"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ling\PycharmProjects\epic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ling/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10365" windowHeight="9630" tabRatio="678" activeTab="4"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="678" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Trade" sheetId="2" r:id="rId1"/>
-    <sheet name="WorkMethod" sheetId="3" r:id="rId2"/>
-    <sheet name="WorkMethodDependency" sheetId="4" r:id="rId3"/>
-    <sheet name="Space" sheetId="5" r:id="rId4"/>
-    <sheet name="Design" sheetId="6" r:id="rId5"/>
+    <sheet name="trade" sheetId="2" r:id="rId1"/>
+    <sheet name="work_method" sheetId="3" r:id="rId2"/>
+    <sheet name="work_method_dependency" sheetId="4" r:id="rId3"/>
+    <sheet name="space" sheetId="5" r:id="rId4"/>
+    <sheet name="design" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="18">
-  <si>
-    <t>WorkMethod</t>
-  </si>
-  <si>
-    <t>WorkSpace</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
   <si>
     <t>trade_1</t>
   </si>
@@ -44,9 +42,6 @@
     <t>trade_3</t>
   </si>
   <si>
-    <t>TradeName</t>
-  </si>
-  <si>
     <t>work_1</t>
   </si>
   <si>
@@ -59,32 +54,44 @@
     <t>work_4</t>
   </si>
   <si>
-    <t>Productivity</t>
-  </si>
-  <si>
-    <t>Method</t>
-  </si>
-  <si>
-    <t>Predecessor</t>
-  </si>
-  <si>
-    <t>Successor</t>
-  </si>
-  <si>
     <t>floor_1</t>
   </si>
   <si>
     <t>floor_2</t>
   </si>
   <si>
-    <t>Quantity</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>trade_name</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>productivity</t>
+  </si>
+  <si>
+    <t>predecessor</t>
+  </si>
+  <si>
+    <t>successor</t>
+  </si>
+  <si>
+    <t>work_method</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>space</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -183,9 +190,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -218,9 +225,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -426,34 +433,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -471,68 +477,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="1023" width="11.5703125"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
       <c r="C3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>6</v>
@@ -553,18 +558,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -572,36 +576,36 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -617,56 +621,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -684,89 +662,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="1024" width="11.5703125"/>
+    <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
       </c>
       <c r="C2">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
       </c>
       <c r="C6">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>20</v>

</xml_diff>

<commit_message>
draw line of balance chart using plotly in jupyter
</commit_message>
<xml_diff>
--- a/epic.xlsx
+++ b/epic.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ling/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ling\PycharmProjects\epic\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="678" activeTab="3"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="28725" windowHeight="17535" tabRatio="678" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="trade" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
   <si>
     <t>trade_1</t>
   </si>
@@ -52,12 +52,6 @@
   </si>
   <si>
     <t>work_4</t>
-  </si>
-  <si>
-    <t>floor_1</t>
-  </si>
-  <si>
-    <t>floor_2</t>
   </si>
   <si>
     <t>name</t>
@@ -90,8 +84,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -437,27 +431,27 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -481,25 +475,25 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -510,7 +504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -521,7 +515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -532,7 +526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -562,21 +556,21 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -584,7 +578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -592,7 +586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -600,7 +594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -623,28 +617,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>8</v>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -662,91 +656,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
       <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
+      <c r="B3">
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
+      <c r="B4">
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
+      <c r="B5">
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
         <v>8</v>
       </c>
-      <c r="C6">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
         <v>8</v>
-      </c>
-      <c r="C7">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
the horizontal line of waiting time was removed in the result data
</commit_message>
<xml_diff>
--- a/epic.xlsx
+++ b/epic.xlsx
@@ -657,7 +657,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -685,7 +685,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -696,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -718,7 +718,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -729,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -740,7 +740,7 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix the bug of multi-constraints problem
</commit_message>
<xml_diff>
--- a/epic.xlsx
+++ b/epic.xlsx
@@ -427,7 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -471,9 +471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
@@ -656,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -685,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -696,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3">

</xml_diff>

<commit_message>
added variability in productivity and quantity of the work
</commit_message>
<xml_diff>
--- a/epic.xlsx
+++ b/epic.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>trade_1</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>space</t>
+  </si>
+  <si>
+    <t>productivity_variation</t>
+  </si>
+  <si>
+    <t>design_variation</t>
   </si>
 </sst>
 </file>
@@ -469,9 +475,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
@@ -480,7 +488,7 @@
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -490,8 +498,11 @@
       <c r="C1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -501,8 +512,11 @@
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -512,8 +526,11 @@
       <c r="C3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -523,8 +540,11 @@
       <c r="C4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -533,6 +553,9 @@
       </c>
       <c r="C5">
         <v>6</v>
+      </c>
+      <c r="D5">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -652,19 +675,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -674,8 +697,11 @@
       <c r="C1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -685,8 +711,11 @@
       <c r="C2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -696,8 +725,11 @@
       <c r="C3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -707,8 +739,11 @@
       <c r="C4">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -718,8 +753,11 @@
       <c r="C5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -729,8 +767,11 @@
       <c r="C6">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -739,6 +780,9 @@
       </c>
       <c r="C7">
         <v>20</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>